<commit_message>
update testcase và báo cáo
</commit_message>
<xml_diff>
--- a/Bao_cao/Test cases.xlsx
+++ b/Bao_cao/Test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" windowWidth="13545" windowHeight="12210"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" windowWidth="27945" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="17" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="134">
   <si>
     <t>CASE</t>
   </si>
@@ -265,19 +265,7 @@
     <t>Create Ingredient</t>
   </si>
   <si>
-    <t>Giới hạn Unit</t>
-  </si>
-  <si>
-    <t>Chỉ cho phép khối lượng từ 100 đến 10000</t>
-  </si>
-  <si>
     <t>Create Topping</t>
-  </si>
-  <si>
-    <t>Giới hạn Price</t>
-  </si>
-  <si>
-    <t>Chỉ cho phép số lượng từ 0 đến 100</t>
   </si>
   <si>
     <t>Create Size</t>
@@ -1600,10 +1588,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:F98"/>
+  <dimension ref="B2:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1" outlineLevelCol="5"/>
@@ -2202,11 +2190,11 @@
         <v>6.2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F44" s="6"/>
     </row>
@@ -2215,712 +2203,673 @@
         <v>6.3</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E45" s="6" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="F45" s="6"/>
     </row>
     <row r="46" customHeight="1" spans="2:6">
-      <c r="B46" s="11">
-        <v>6.4</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="6"/>
+      <c r="B46" s="2">
+        <v>7</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" customHeight="1" spans="2:6">
-      <c r="B47" s="2">
+      <c r="B47" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="F47" s="6"/>
     </row>
     <row r="48" customHeight="1" spans="2:6">
       <c r="B48" s="11">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="F48" s="6"/>
     </row>
     <row r="49" customHeight="1" spans="2:6">
       <c r="B49" s="11">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E49" s="6" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="F49" s="6"/>
     </row>
     <row r="50" customHeight="1" spans="2:6">
-      <c r="B50" s="11">
-        <v>7.3</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50" s="6"/>
+      <c r="B50" s="2">
+        <v>8</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" customHeight="1" spans="2:6">
       <c r="B51" s="11">
-        <v>7.4</v>
+        <v>8.1</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D51" s="6"/>
       <c r="E51" s="6" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F51" s="6"/>
     </row>
     <row r="52" customHeight="1" spans="2:6">
-      <c r="B52" s="2">
-        <v>8</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="B52" s="11">
+        <v>8.2</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" customHeight="1" spans="2:6">
       <c r="B53" s="11">
-        <v>8.1</v>
+        <v>8.3</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D53" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E53" s="6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F53" s="6"/>
     </row>
     <row r="54" customHeight="1" spans="2:6">
-      <c r="B54" s="11">
-        <v>8.2</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F54" s="6"/>
+      <c r="B54" s="2">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" customHeight="1" spans="2:6">
       <c r="B55" s="11">
-        <v>8.3</v>
+        <v>9.1</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F55" s="6"/>
     </row>
     <row r="56" customHeight="1" spans="2:6">
       <c r="B56" s="11">
-        <v>8.4</v>
+        <v>9.2</v>
       </c>
       <c r="C56" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" customHeight="1" spans="2:6">
+      <c r="B57" s="11">
+        <v>9.3</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E57" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" customHeight="1" spans="2:6">
-      <c r="B57" s="2">
-        <v>9</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" customHeight="1" spans="2:6">
-      <c r="B58" s="11">
-        <v>9.1</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="6"/>
+      <c r="B58" s="2">
+        <v>10</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="59" customHeight="1" spans="2:6">
       <c r="B59" s="11">
-        <v>9.2</v>
+        <v>10.1</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F59" s="6"/>
     </row>
     <row r="60" customHeight="1" spans="2:6">
       <c r="B60" s="11">
-        <v>9.3</v>
+        <v>10.2</v>
       </c>
       <c r="C60" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" customHeight="1" spans="2:6">
+      <c r="B61" s="11">
+        <v>10.3</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E61" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="6"/>
-    </row>
-    <row r="61" customHeight="1" spans="2:6">
-      <c r="B61" s="2">
-        <v>10</v>
-      </c>
-      <c r="C61" s="3" t="s">
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" customHeight="1" spans="2:6">
+      <c r="B62" s="2">
+        <v>11</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+    </row>
+    <row r="63" customHeight="1" spans="2:6">
+      <c r="B63" s="5">
+        <v>11.1</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" customHeight="1" spans="2:6">
+      <c r="B64" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-    </row>
-    <row r="62" customHeight="1" spans="2:6">
-      <c r="B62" s="11">
-        <v>10.1</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" customHeight="1" spans="2:6">
-      <c r="B63" s="11">
-        <v>10.2</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F63" s="6"/>
-    </row>
-    <row r="64" customHeight="1" spans="2:6">
-      <c r="B64" s="11">
-        <v>10.3</v>
-      </c>
-      <c r="C64" s="6" t="s">
+      <c r="D64" s="7"/>
+      <c r="E64" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" customHeight="1" spans="2:6">
+      <c r="B65" s="11">
+        <v>11.3</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D65" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E65" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" customHeight="1" spans="2:6">
-      <c r="B65" s="2">
-        <v>11</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
+      <c r="F65" s="6"/>
     </row>
     <row r="66" customHeight="1" spans="2:6">
-      <c r="B66" s="5">
-        <v>11.1</v>
-      </c>
-      <c r="C66" s="7" t="s">
+      <c r="B66" s="14">
+        <v>12</v>
+      </c>
+      <c r="C66" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
     </row>
     <row r="67" customHeight="1" spans="2:6">
       <c r="B67" s="5">
-        <v>11.2</v>
+        <v>12.1</v>
       </c>
       <c r="C67" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" customHeight="1" spans="2:6">
+      <c r="B68" s="5">
+        <v>12.2</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F67" s="7"/>
-    </row>
-    <row r="68" customHeight="1" spans="2:6">
-      <c r="B68" s="11">
-        <v>11.3</v>
-      </c>
-      <c r="C68" s="6" t="s">
+      <c r="D68" s="7"/>
+      <c r="E68" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" customHeight="1" spans="2:6">
+      <c r="B69" s="11">
+        <v>12.3</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="E69" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" customHeight="1" spans="2:6">
-      <c r="B69" s="14">
-        <v>12</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" customHeight="1" spans="2:6">
-      <c r="B70" s="5">
-        <v>12.1</v>
-      </c>
-      <c r="C70" s="7" t="s">
+      <c r="B70" s="14">
+        <v>13</v>
+      </c>
+      <c r="C70" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
     </row>
     <row r="71" customHeight="1" spans="2:6">
       <c r="B71" s="5">
-        <v>12.2</v>
+        <v>13.1</v>
       </c>
       <c r="C71" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7" t="s">
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" customHeight="1" spans="2:6">
+      <c r="B72" s="5">
+        <v>13.2</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" customHeight="1" spans="2:6">
-      <c r="B72" s="11">
+      <c r="D72" s="7"/>
+      <c r="E72" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" customHeight="1" spans="2:6">
+      <c r="B73" s="11">
         <v>12.3</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C73" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E73" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F72" s="6"/>
-    </row>
-    <row r="73" customHeight="1" spans="2:6">
-      <c r="B73" s="14">
-        <v>13</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
+      <c r="F73" s="6"/>
     </row>
     <row r="74" customHeight="1" spans="2:6">
-      <c r="B74" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="C74" s="7" t="s">
+      <c r="B74" s="14">
+        <v>14</v>
+      </c>
+      <c r="C74" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E74" s="7"/>
-      <c r="F74" s="7"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
     </row>
     <row r="75" customHeight="1" spans="2:6">
       <c r="B75" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" customHeight="1" spans="2:6">
+      <c r="B76" s="5">
         <v>13.2</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C76" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7" t="s">
+      <c r="D76" s="7"/>
+      <c r="E76" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F75" s="7"/>
-    </row>
-    <row r="76" customHeight="1" spans="2:6">
-      <c r="B76" s="11">
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" customHeight="1" spans="2:6">
+      <c r="B77" s="11">
         <v>12.3</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C77" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D77" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E77" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F76" s="6"/>
-    </row>
-    <row r="77" customHeight="1" spans="2:6">
-      <c r="B77" s="14">
-        <v>14</v>
-      </c>
-      <c r="C77" s="15" t="s">
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" customHeight="1" spans="2:6">
+      <c r="B78" s="14">
+        <v>15</v>
+      </c>
+      <c r="C78" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-    </row>
-    <row r="78" customHeight="1" spans="2:6">
-      <c r="B78" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
     </row>
     <row r="79" customHeight="1" spans="2:6">
       <c r="B79" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" customHeight="1" spans="2:6">
+      <c r="B80" s="5">
         <v>13.2</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="80" customHeight="1" spans="2:6">
-      <c r="B80" s="11">
+      <c r="D80" s="7"/>
+      <c r="E80" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" customHeight="1" spans="2:6">
+      <c r="B81" s="11">
         <v>12.3</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C81" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" customHeight="1" spans="2:6">
-      <c r="B81" s="14">
-        <v>15</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="16"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" customHeight="1" spans="2:6">
-      <c r="B82" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="C82" s="7" t="s">
+      <c r="B82" s="14">
+        <v>16</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D82" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
     </row>
     <row r="83" customHeight="1" spans="2:6">
       <c r="B83" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" customHeight="1" spans="2:6">
+      <c r="B84" s="5">
         <v>13.2</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7" t="s">
+      <c r="C84" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F83" s="7"/>
-    </row>
-    <row r="84" customHeight="1" spans="2:6">
-      <c r="B84" s="11">
+      <c r="D84" s="7"/>
+      <c r="E84" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" customHeight="1" spans="2:6">
+      <c r="B85" s="11">
         <v>12.3</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C85" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D85" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E84" s="6" t="s">
+      <c r="E85" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="6"/>
-    </row>
-    <row r="85" customHeight="1" spans="2:6">
-      <c r="B85" s="14">
-        <v>16</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" customHeight="1" spans="2:6">
-      <c r="B86" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="C86" s="7" t="s">
+      <c r="B86" s="14">
+        <v>17</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D86" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
     </row>
     <row r="87" customHeight="1" spans="2:6">
       <c r="B87" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" customHeight="1" spans="2:6">
+      <c r="B88" s="5">
         <v>13.2</v>
       </c>
-      <c r="C87" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7" t="s">
+      <c r="C88" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F87" s="7"/>
-    </row>
-    <row r="88" customHeight="1" spans="2:6">
-      <c r="B88" s="11">
+      <c r="D88" s="7"/>
+      <c r="E88" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" customHeight="1" spans="2:6">
+      <c r="B89" s="11">
         <v>12.3</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C89" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D89" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="E89" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F88" s="6"/>
-    </row>
-    <row r="89" customHeight="1" spans="2:6">
-      <c r="B89" s="14">
-        <v>17</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D89" s="16"/>
-      <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
+      <c r="F89" s="6"/>
     </row>
     <row r="90" customHeight="1" spans="2:6">
-      <c r="B90" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="C90" s="7" t="s">
+      <c r="B90" s="14">
+        <v>18</v>
+      </c>
+      <c r="C90" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
     </row>
     <row r="91" customHeight="1" spans="2:6">
       <c r="B91" s="5">
-        <v>13.2</v>
+        <v>18.1</v>
       </c>
       <c r="C91" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D91" s="7"/>
       <c r="E91" s="7" t="s">
         <v>124</v>
       </c>
       <c r="F91" s="7"/>
     </row>
     <row r="92" customHeight="1" spans="2:6">
-      <c r="B92" s="11">
-        <v>12.3</v>
-      </c>
-      <c r="C92" s="6" t="s">
+      <c r="B92" s="5">
+        <v>18.2</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" customHeight="1" spans="2:6">
+      <c r="B93" s="11">
+        <v>18.3</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" customHeight="1" spans="2:6">
+      <c r="B94" s="11">
+        <v>18.4</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" customHeight="1" spans="2:6">
+      <c r="B95" s="11">
+        <v>18.3</v>
+      </c>
+      <c r="C95" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D92" s="6" t="s">
+      <c r="D95" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E92" s="6" t="s">
+      <c r="E95" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="6"/>
-    </row>
-    <row r="93" customHeight="1" spans="2:6">
-      <c r="B93" s="14">
-        <v>18</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D93" s="16"/>
-      <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
-    </row>
-    <row r="94" customHeight="1" spans="2:6">
-      <c r="B94" s="5">
-        <v>18.1</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" customHeight="1" spans="2:6">
-      <c r="B95" s="5">
-        <v>18.2</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F95" s="7"/>
-    </row>
-    <row r="96" customHeight="1" spans="2:6">
-      <c r="B96" s="11">
-        <v>18.3</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F96" s="6"/>
-    </row>
-    <row r="97" customHeight="1" spans="2:6">
-      <c r="B97" s="11">
-        <v>18.4</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F97" s="6"/>
-    </row>
-    <row r="98" customHeight="1" spans="2:6">
-      <c r="B98" s="11">
-        <v>18.3</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F98" s="6"/>
+      <c r="F95" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>